<commit_message>
update excel dummy data
</commit_message>
<xml_diff>
--- a/scriptDatabase/quarantined_person.xlsx
+++ b/scriptDatabase/quarantined_person.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\UIT\Nam 3\HKI\PP OOP\Project\QuanLyKhuCachLy\scriptDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E10C1EB-9AED-4270-A585-23E7042A324E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D02C214-5631-495C-834B-D155AD251579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{53B6D07A-B72C-4875-A261-E7F84EEB7438}"/>
   </bookViews>
@@ -529,15 +529,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CD999E-6D30-4CC0-AB9A-DF9962F9583E}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
     <col min="13" max="13" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1114,7 +1120,7 @@
         <v>17</v>
       </c>
       <c r="M15" s="1">
-        <v>44516</v>
+        <v>44517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>